<commit_message>
Update communion columns added
</commit_message>
<xml_diff>
--- a/public/forms/first-communion-format.xlsx
+++ b/public/forms/first-communion-format.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Macoy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\church-mis\public\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3519F17-5E95-4FA4-B361-0E79EADF1128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E828BE6-BA33-4FC7-B477-EB89565830F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AF45597-10AB-400D-B240-38F312BD0E22}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AF45597-10AB-400D-B240-38F312BD0E22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Present Address</t>
   </si>
   <si>
-    <t>Guardian</t>
-  </si>
-  <si>
     <t>John Mark Victorino</t>
   </si>
   <si>
@@ -58,6 +55,27 @@
   </si>
   <si>
     <t>Kyla Faith Victorino</t>
+  </si>
+  <si>
+    <t>Mother</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Sarah Lee</t>
+  </si>
+  <si>
+    <t>Sponsor 1</t>
+  </si>
+  <si>
+    <t>Sponsor 2</t>
+  </si>
+  <si>
+    <t>Richard Bowers</t>
+  </si>
+  <si>
+    <t>Mikee Corbito</t>
   </si>
 </sst>
 </file>
@@ -66,7 +84,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="167" formatCode="00000000000"/>
+    <numFmt numFmtId="165" formatCode="00000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -113,11 +131,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,7 +164,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1004395</xdr:rowOff>
     </xdr:to>
@@ -481,29 +499,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670E7318-4698-4C2F-93B7-823947330421}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="2" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+    <row r="1" spans="1:10" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -511,88 +532,133 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="B3" s="3">
+        <v>34899</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4">
+        <v>9062268483</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>34899</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4">
+        <v>9062268483</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
         <v>34899</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="4">
+        <v>9062268483</v>
+      </c>
+      <c r="H5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>34899</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4">
         <v>9062268483</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4">
-        <v>34899</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="H6" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" s="5">
-        <v>9062268483</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4">
-        <v>34899</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5">
-        <v>9062268483</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4">
-        <v>34899</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="5">
-        <v>9062268483</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>